<commit_message>
hand made markov chain
</commit_message>
<xml_diff>
--- a/weekly-percent-increase.xlsx
+++ b/weekly-percent-increase.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>weekly newv4linksperc</t>
   </si>
@@ -78,6 +78,9 @@
   <si>
     <t>week</t>
   </si>
+  <si>
+    <t>IPv6-probability</t>
+  </si>
 </sst>
 </file>
 
@@ -125,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -213,11 +216,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,6 +337,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2911,7 +3014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G17" workbookViewId="0">
+      <selection activeCell="X32" sqref="X32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4862,7 +4967,7 @@
         <v>6-7</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="5"/>
         <v>27</v>
@@ -4890,7 +4995,7 @@
         <v>3-4</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="5"/>
         <v>28</v>
@@ -4917,34 +5022,34 @@
         <f t="shared" si="7"/>
         <v>5-6</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="12" t="s">
+      <c r="I30" s="20"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="6"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA30" s="5"/>
-      <c r="AB30" s="5"/>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
-      <c r="AE30" s="5"/>
-      <c r="AF30" s="5"/>
-      <c r="AG30" s="6"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="23"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="21"/>
+      <c r="Z30" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA30" s="21"/>
+      <c r="AB30" s="21"/>
+      <c r="AC30" s="21"/>
+      <c r="AD30" s="21"/>
+      <c r="AE30" s="21"/>
+      <c r="AF30" s="21"/>
+      <c r="AG30" s="23"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -4973,7 +5078,7 @@
         <f t="shared" si="7"/>
         <v>4-5</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -4986,8 +5091,8 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
-      <c r="T31" s="9"/>
-      <c r="V31" s="7"/>
+      <c r="T31" s="25"/>
+      <c r="V31" s="24"/>
       <c r="W31" s="8"/>
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
@@ -5000,7 +5105,7 @@
       <c r="AD31" s="8"/>
       <c r="AE31" s="8"/>
       <c r="AF31" s="8"/>
-      <c r="AG31" s="9"/>
+      <c r="AG31" s="25"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -5029,7 +5134,7 @@
         <f t="shared" si="7"/>
         <v>3-4</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="8"/>
       <c r="K32" s="13" t="str">
         <f t="array" ref="K32:T32">TRANSPOSE($M$2:$M$11)</f>
@@ -5059,10 +5164,10 @@
       <c r="S32" s="13" t="str">
         <v>16-18</v>
       </c>
-      <c r="T32" s="14" t="str">
+      <c r="T32" s="26" t="str">
         <v>18-up</v>
       </c>
-      <c r="V32" s="7"/>
+      <c r="V32" s="24"/>
       <c r="W32" s="8"/>
       <c r="X32" s="13" t="str">
         <f t="array" ref="X32:AG32">TRANSPOSE($P$2:$P$11)</f>
@@ -5092,7 +5197,7 @@
       <c r="AF32" s="13" t="str">
         <v>8-9</v>
       </c>
-      <c r="AG32" s="14" t="str">
+      <c r="AG32" s="26" t="str">
         <v>9-up</v>
       </c>
     </row>
@@ -5123,7 +5228,7 @@
         <f t="shared" si="7"/>
         <v>3-4</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="24"/>
       <c r="J33" s="8" t="str">
         <f t="array" ref="J33:J42">$M$2:$M$11</f>
         <v>0-2</v>
@@ -5164,11 +5269,11 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="T33" s="16">
+      <c r="T33" s="27">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="V33" s="7"/>
+      <c r="V33" s="24"/>
       <c r="W33" s="8" t="str">
         <f t="array" ref="W33:W42">$P$2:$P$11</f>
         <v>0-1</v>
@@ -5209,7 +5314,7 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AG33" s="16">
+      <c r="AG33" s="27">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -5233,7 +5338,7 @@
         <f t="shared" si="7"/>
         <v>4-5</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="24"/>
       <c r="J34" s="8" t="str">
         <v>2-4</v>
       </c>
@@ -5273,11 +5378,11 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="T34" s="16">
+      <c r="T34" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V34" s="7"/>
+      <c r="V34" s="24"/>
       <c r="W34" s="8" t="str">
         <v>1-2</v>
       </c>
@@ -5317,7 +5422,7 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AG34" s="16">
+      <c r="AG34" s="27">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -5341,7 +5446,7 @@
         <f t="shared" si="7"/>
         <v>7-8</v>
       </c>
-      <c r="I35" s="7"/>
+      <c r="I35" s="24"/>
       <c r="J35" s="8" t="str">
         <v>4-6</v>
       </c>
@@ -5381,11 +5486,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="T35" s="16">
+      <c r="T35" s="27">
         <f t="shared" si="16"/>
         <v>0.125</v>
       </c>
-      <c r="V35" s="7"/>
+      <c r="V35" s="24"/>
       <c r="W35" s="8" t="str">
         <v>2-3</v>
       </c>
@@ -5425,7 +5530,7 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AG35" s="16">
+      <c r="AG35" s="27">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
@@ -5449,7 +5554,7 @@
         <f t="shared" si="7"/>
         <v>3-4</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="24"/>
       <c r="J36" s="8" t="str">
         <v>6-8</v>
       </c>
@@ -5489,11 +5594,11 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="T36" s="16">
+      <c r="T36" s="27">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="V36" s="7"/>
+      <c r="V36" s="24"/>
       <c r="W36" s="8" t="str">
         <v>3-4</v>
       </c>
@@ -5533,7 +5638,7 @@
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="AG36" s="16">
+      <c r="AG36" s="27">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -5557,7 +5662,7 @@
         <f t="shared" si="7"/>
         <v>4-5</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I37" s="24" t="s">
         <v>10</v>
       </c>
       <c r="J37" s="8" t="str">
@@ -5599,11 +5704,11 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T37" s="16">
+      <c r="T37" s="27">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="V37" s="7" t="s">
+      <c r="V37" s="24" t="s">
         <v>10</v>
       </c>
       <c r="W37" s="8" t="str">
@@ -5645,7 +5750,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AG37" s="16">
+      <c r="AG37" s="27">
         <f t="shared" si="21"/>
         <v>0.33333333333333331</v>
       </c>
@@ -5669,7 +5774,7 @@
         <f t="shared" si="7"/>
         <v>9-up</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="8" t="str">
         <v>10-12</v>
       </c>
@@ -5709,11 +5814,11 @@
         <f t="shared" si="22"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="T38" s="16">
+      <c r="T38" s="27">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V38" s="7"/>
+      <c r="V38" s="24"/>
       <c r="W38" s="8" t="str">
         <v>5-6</v>
       </c>
@@ -5753,7 +5858,7 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AG38" s="16">
+      <c r="AG38" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -5781,7 +5886,7 @@
         <f t="shared" si="7"/>
         <v>8-9</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="24"/>
       <c r="J39" s="8" t="str">
         <v>12-14</v>
       </c>
@@ -5821,11 +5926,11 @@
         <f t="shared" si="24"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="T39" s="16">
+      <c r="T39" s="27">
         <f t="shared" si="24"/>
         <v>0.75</v>
       </c>
-      <c r="V39" s="7"/>
+      <c r="V39" s="24"/>
       <c r="W39" s="8" t="str">
         <v>6-7</v>
       </c>
@@ -5865,7 +5970,7 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="AG39" s="16">
+      <c r="AG39" s="27">
         <f t="shared" si="25"/>
         <v>0.33333333333333331</v>
       </c>
@@ -5897,7 +6002,7 @@
         <f t="shared" si="7"/>
         <v>3-4</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="24"/>
       <c r="J40" s="8" t="str">
         <v>14-16</v>
       </c>
@@ -5937,11 +6042,11 @@
         <f t="shared" si="26"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="T40" s="16">
+      <c r="T40" s="27">
         <f t="shared" si="26"/>
         <v>0.125</v>
       </c>
-      <c r="V40" s="7"/>
+      <c r="V40" s="24"/>
       <c r="W40" s="8" t="str">
         <v>7-8</v>
       </c>
@@ -5981,7 +6086,7 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AG40" s="16">
+      <c r="AG40" s="27">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
@@ -6013,7 +6118,7 @@
         <f t="shared" si="7"/>
         <v>3-4</v>
       </c>
-      <c r="I41" s="7"/>
+      <c r="I41" s="24"/>
       <c r="J41" s="8" t="str">
         <v>16-18</v>
       </c>
@@ -6053,11 +6158,11 @@
         <f t="shared" si="29"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="T41" s="16">
+      <c r="T41" s="27">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="V41" s="7"/>
+      <c r="V41" s="24"/>
       <c r="W41" s="8" t="str">
         <v>8-9</v>
       </c>
@@ -6097,12 +6202,12 @@
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AG41" s="16">
+      <c r="AG41" s="27">
         <f t="shared" si="30"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="5"/>
         <v>40</v>
@@ -6129,96 +6234,96 @@
         <f t="shared" si="7"/>
         <v>5-6</v>
       </c>
-      <c r="I42" s="10"/>
-      <c r="J42" s="11" t="str">
+      <c r="I42" s="28"/>
+      <c r="J42" s="29" t="str">
         <v>18-up</v>
       </c>
-      <c r="K42" s="17" t="e">
+      <c r="K42" s="30" t="e">
         <f t="shared" ref="K42:T42" si="31">K27/SUM(K$18:K$27)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L42" s="17" t="e">
+      <c r="L42" s="30" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M42" s="17">
+      <c r="M42" s="30">
         <f t="shared" si="31"/>
         <v>1</v>
       </c>
-      <c r="N42" s="17" t="e">
+      <c r="N42" s="30" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O42" s="17" t="e">
+      <c r="O42" s="30" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P42" s="17">
+      <c r="P42" s="30">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="Q42" s="30">
         <f t="shared" si="31"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="R42" s="17">
+      <c r="R42" s="30">
         <f t="shared" si="31"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="S42" s="17">
+      <c r="S42" s="30">
         <f t="shared" si="31"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="T42" s="18">
+      <c r="T42" s="31">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="V42" s="10"/>
-      <c r="W42" s="11" t="str">
+      <c r="V42" s="28"/>
+      <c r="W42" s="29" t="str">
         <v>9-up</v>
       </c>
-      <c r="X42" s="17" t="e">
+      <c r="X42" s="30" t="e">
         <f t="shared" ref="X42:AG42" si="32">X27/SUM(X$18:X$27)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y42" s="17" t="e">
+      <c r="Y42" s="30" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z42" s="17">
+      <c r="Z42" s="30">
         <f t="shared" si="32"/>
         <v>0.5</v>
       </c>
-      <c r="AA42" s="17">
+      <c r="AA42" s="30">
         <f t="shared" si="32"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AB42" s="17">
+      <c r="AB42" s="30">
         <f t="shared" si="32"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="AC42" s="17">
+      <c r="AC42" s="30">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AD42" s="17">
+      <c r="AD42" s="30">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AE42" s="17">
+      <c r="AE42" s="30">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AF42" s="17">
+      <c r="AF42" s="30">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AG42" s="18">
+      <c r="AG42" s="31">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="5"/>
         <v>41</v>

</xml_diff>